<commit_message>
update car_parts_script and bat
better output structure in cmd and part
</commit_message>
<xml_diff>
--- a/part.xlsx
+++ b/part.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\car_parts_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mizx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EFD8B6-0C4E-43C8-9BE9-0E3722A10FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8EDF96-B03A-423A-9F7B-11C792FACDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,30 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="210">
   <si>
     <t>Марка</t>
   </si>
@@ -637,13 +615,67 @@
   </si>
   <si>
     <t>PRG</t>
+  </si>
+  <si>
+    <t>VOLVO</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Вес нетто</t>
+  </si>
+  <si>
+    <t>Материал</t>
+  </si>
+  <si>
+    <t>КОРРЕКТНЫЕ МАРКИ</t>
+  </si>
+  <si>
+    <t>Ссылка</t>
+  </si>
+  <si>
+    <t>8972564 STDB</t>
+  </si>
+  <si>
+    <t>8971533 STD</t>
+  </si>
+  <si>
+    <t>4049337 H</t>
+  </si>
+  <si>
+    <t>1971P060 STD</t>
+  </si>
+  <si>
+    <t>PRO1220040</t>
+  </si>
+  <si>
+    <t>KS00000031</t>
+  </si>
+  <si>
+    <t>NÜRAL</t>
+  </si>
+  <si>
+    <t>HOLSET</t>
+  </si>
+  <si>
+    <t>MİBA</t>
+  </si>
+  <si>
+    <t>FEBİ</t>
+  </si>
+  <si>
+    <t>PACCAR</t>
+  </si>
+  <si>
+    <t>PROVIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,8 +728,15 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,8 +749,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -734,6 +779,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -744,23 +804,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -772,13 +826,25 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 5" xfId="4" xr:uid="{8109BDE5-1BD8-4322-AD7D-F394A8C5CDA1}"/>
     <cellStyle name="Normal 20" xfId="3" xr:uid="{5849B991-F21B-4D6D-9BAB-C19B5059C54E}"/>
     <cellStyle name="Normal 22" xfId="5" xr:uid="{072F34E1-8FEA-43A7-BE6D-EC33D993FD69}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{A386A9A2-73E0-47D5-94CE-710A2900268B}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="6" xr:uid="{62A7680B-80E5-47A8-B3C8-1FC89DB158EA}"/>
     <cellStyle name="Обычный 3" xfId="1" xr:uid="{2DCA1B57-3B79-4B40-A56B-6ACAB7C28A68}"/>
   </cellStyles>
@@ -1059,40 +1125,136 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="21.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="str" cm="1">
-        <f t="array" ref="C1">IF(A1="Артикул","ОЧИСТКА АРТИКУЛА",TRIM(SUBSTITUTE(UPPER(A1),INDEX(UPPER('МАРКИ ДЛЯ ЧИСТКИ'!A:A),MATCH(TRUE,ISNUMBER(FIND(UPPER('МАРКИ ДЛЯ ЧИСТКИ'!A:A),UPPER(A1))),0)),"")))</f>
-        <v>ОЧИСТКА АРТИКУЛА</v>
-      </c>
-      <c r="D1" s="2" cm="1">
-        <f t="array" ref="D1">IFERROR(INDEX('МАРКИ ДЛЯ ЧИСТКИ'!A:A,MATCH(TRUE,SEARCH('МАРКИ ДЛЯ ЧИСТКИ'!A:A,A1)&gt;0,0)),"")</f>
-        <v>0</v>
+      <c r="C1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>71259</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>23617501</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>1948921</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>1699168</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>1161251</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1117,119 +1279,119 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B62" si="0">LEN(A2)</f>
         <v>17</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B13">
@@ -1238,7 +1400,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14">
@@ -1247,7 +1409,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B15">
@@ -1256,7 +1418,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B16">
@@ -1265,7 +1427,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B17">
@@ -1274,7 +1436,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B18">
@@ -1283,7 +1445,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B19">
@@ -1292,7 +1454,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B20">
@@ -1301,7 +1463,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B21">
@@ -1310,7 +1472,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>156</v>
       </c>
       <c r="B22">
@@ -1319,7 +1481,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B23">
@@ -1328,7 +1490,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B24">
@@ -1337,7 +1499,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B25">
@@ -1346,7 +1508,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B26">
@@ -1355,7 +1517,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B27">
@@ -1364,7 +1526,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B28">
@@ -1373,7 +1535,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B29">
@@ -1382,7 +1544,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B30">
@@ -1391,7 +1553,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B31">
@@ -1400,7 +1562,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>160</v>
       </c>
       <c r="B32">
@@ -1409,7 +1571,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B33">
@@ -1418,7 +1580,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B34">
@@ -1427,7 +1589,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -1436,7 +1598,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B36">
@@ -1445,7 +1607,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B37">
@@ -1454,7 +1616,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B38">
@@ -1463,7 +1625,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B39">
@@ -1472,7 +1634,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B40">
@@ -1481,7 +1643,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B41">
@@ -1490,7 +1652,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B42">
@@ -1499,7 +1661,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B43">
@@ -1508,7 +1670,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B44">
@@ -1517,7 +1679,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B45">
@@ -1526,7 +1688,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B46">
@@ -1535,7 +1697,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B47">
@@ -1544,41 +1706,41 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="8" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D49" s="10"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="8" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B51">
@@ -1587,7 +1749,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B52">
@@ -1596,7 +1758,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B53">
@@ -1605,7 +1767,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B54">
@@ -1614,7 +1776,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B55">
@@ -1623,7 +1785,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B56">
@@ -1632,7 +1794,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B57">
@@ -1641,7 +1803,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B58">
@@ -1650,7 +1812,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B59">
@@ -1659,7 +1821,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B60">
@@ -1668,7 +1830,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B61">
@@ -1677,7 +1839,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B62">
@@ -1686,7 +1848,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B63">
@@ -1695,7 +1857,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B64">
@@ -1704,7 +1866,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B65">
@@ -1713,7 +1875,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B66">
@@ -1722,7 +1884,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B67">
@@ -1731,7 +1893,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B68">
@@ -1740,7 +1902,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B69">
@@ -1749,7 +1911,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B70">
@@ -1758,7 +1920,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B71">
@@ -1767,7 +1929,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B72">
@@ -1776,7 +1938,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B73">
@@ -1785,7 +1947,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B74">
@@ -1794,7 +1956,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B75">
@@ -1803,7 +1965,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B76">
@@ -1812,7 +1974,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B77">
@@ -1821,7 +1983,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>184</v>
       </c>
       <c r="B78">
@@ -1830,7 +1992,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B79">
@@ -1839,7 +2001,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B80">
@@ -1848,7 +2010,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B81">
@@ -1857,7 +2019,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B82">
@@ -1866,7 +2028,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B83">
@@ -1875,7 +2037,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B84">
@@ -1884,7 +2046,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B85">
@@ -1893,7 +2055,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B86">
@@ -1902,7 +2064,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B87">
@@ -1911,7 +2073,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B88">
@@ -1920,7 +2082,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B89">
@@ -1929,7 +2091,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B90">
@@ -1938,7 +2100,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B91">
@@ -1947,7 +2109,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B92">
@@ -1956,7 +2118,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B93">
@@ -1965,7 +2127,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B94">
@@ -1974,7 +2136,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B95">
@@ -1983,7 +2145,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B96">
@@ -1992,7 +2154,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B97">
@@ -2001,7 +2163,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B98">
@@ -2010,7 +2172,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B99">
@@ -2019,7 +2181,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B100">
@@ -2028,7 +2190,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="4" t="s">
         <v>182</v>
       </c>
       <c r="B101">
@@ -2037,7 +2199,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B102">
@@ -2046,19 +2208,19 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D103" s="10" t="s">
+      <c r="D103" s="8" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B104">
@@ -2067,7 +2229,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B105">
@@ -2076,7 +2238,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B106">
@@ -2085,7 +2247,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B107">
@@ -2094,7 +2256,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B108">
@@ -2103,7 +2265,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B109">
@@ -2112,7 +2274,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B110">
@@ -2121,7 +2283,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B111">
@@ -2130,7 +2292,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B112">
@@ -2139,7 +2301,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B113">
@@ -2148,7 +2310,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B114">
@@ -2157,7 +2319,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B115">
@@ -2166,7 +2328,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B116">
@@ -2175,7 +2337,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B117">
@@ -2184,7 +2346,7 @@
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B118">
@@ -2193,7 +2355,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B119">
@@ -2202,7 +2364,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B120">
@@ -2211,7 +2373,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B121">
@@ -2220,7 +2382,7 @@
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B122">
@@ -2229,7 +2391,7 @@
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B123">
@@ -2238,7 +2400,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B124">
@@ -2247,7 +2409,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="3" t="s">
         <v>180</v>
       </c>
       <c r="B125">
@@ -2256,7 +2418,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B126">
@@ -2265,7 +2427,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B127">
@@ -2274,7 +2436,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B128">
@@ -2283,7 +2445,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B129">
@@ -2292,7 +2454,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B130">
@@ -2301,7 +2463,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B131">
@@ -2310,7 +2472,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="5" t="s">
+      <c r="A132" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B132">
@@ -2319,7 +2481,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="5" t="s">
+      <c r="A133" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B133">
@@ -2328,7 +2490,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B134">
@@ -2337,7 +2499,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="5" t="s">
+      <c r="A135" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B135">
@@ -2346,7 +2508,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="5" t="s">
+      <c r="A136" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B136">
@@ -2355,7 +2517,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B137">
@@ -2364,31 +2526,31 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B138">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D138" s="10" t="s">
+      <c r="D138" s="8" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B139">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D139" s="10" t="s">
+      <c r="D139" s="8" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B140">
@@ -2397,7 +2559,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B141">
@@ -2406,7 +2568,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B142">
@@ -2415,7 +2577,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B143">
@@ -2424,7 +2586,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B144">
@@ -2433,7 +2595,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" s="4" t="s">
+      <c r="A145" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B145">
@@ -2442,7 +2604,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
+      <c r="A146" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B146">
@@ -2451,7 +2613,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="4" t="s">
+      <c r="A147" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B147">
@@ -2460,7 +2622,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="4" t="s">
+      <c r="A148" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B148">
@@ -2469,7 +2631,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" s="4" t="s">
+      <c r="A149" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B149">
@@ -2478,7 +2640,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" s="4" t="s">
+      <c r="A150" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B150">
@@ -2487,7 +2649,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" s="4" t="s">
+      <c r="A151" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B151">
@@ -2496,7 +2658,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" s="5" t="s">
+      <c r="A152" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B152">
@@ -2505,7 +2667,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="5" t="s">
+      <c r="A153" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B153">
@@ -2514,77 +2676,77 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="9" t="s">
+      <c r="A154" s="7" t="s">
         <v>166</v>
       </c>
       <c r="B154">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D154" s="10" t="s">
+      <c r="D154" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" s="9" t="s">
+      <c r="A155" s="7" t="s">
         <v>179</v>
       </c>
       <c r="B155">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D155" s="10"/>
+      <c r="D155" s="8"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="4" t="s">
+      <c r="A156" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B156">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D156" s="10" t="s">
+      <c r="D156" s="8" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B157">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D157" s="10" t="s">
+      <c r="D157" s="8" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" s="4" t="s">
+      <c r="A158" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B158">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D158" s="10" t="s">
+      <c r="D158" s="8" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
+      <c r="A159" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B159">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D159" s="10" t="s">
+      <c r="D159" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="4" t="s">
+      <c r="A160" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B160">
@@ -2593,7 +2755,7 @@
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="4" t="s">
+      <c r="A161" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B161">
@@ -2602,7 +2764,7 @@
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="4" t="s">
+      <c r="A162" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B162">
@@ -2611,7 +2773,7 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
+      <c r="A163" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B163">
@@ -2620,7 +2782,7 @@
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="4" t="s">
+      <c r="A164" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B164">
@@ -2629,7 +2791,7 @@
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="4" t="s">
+      <c r="A165" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B165">
@@ -2638,7 +2800,7 @@
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="4" t="s">
+      <c r="A166" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B166">
@@ -2647,7 +2809,7 @@
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="4" t="s">
+      <c r="A167" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B167">
@@ -2656,7 +2818,7 @@
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="4" t="s">
+      <c r="A168" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B168">
@@ -2665,7 +2827,7 @@
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="4" t="s">
+      <c r="A169" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B169">
@@ -2674,7 +2836,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B170">
@@ -2683,7 +2845,7 @@
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="4" t="s">
+      <c r="A171" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B171">
@@ -2692,7 +2854,7 @@
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="4" t="s">
+      <c r="A172" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B172">
@@ -2701,7 +2863,7 @@
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="4" t="s">
+      <c r="A173" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B173">
@@ -2710,7 +2872,7 @@
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="4" t="s">
+      <c r="A174" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B174">
@@ -2719,7 +2881,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="4" t="s">
+      <c r="A175" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B175">
@@ -2728,7 +2890,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="4" t="s">
+      <c r="A176" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B176">
@@ -2737,7 +2899,7 @@
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="4" t="s">
+      <c r="A177" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B177">
@@ -2746,7 +2908,7 @@
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="4" t="s">
+      <c r="A178" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B178">
@@ -2755,7 +2917,7 @@
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="4" t="s">
+      <c r="A179" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B179">
@@ -2764,7 +2926,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="4" t="s">
+      <c r="A180" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B180">
@@ -2773,7 +2935,7 @@
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B181">
@@ -2782,7 +2944,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="4" t="s">
+      <c r="A182" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B182">
@@ -2791,7 +2953,7 @@
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="4" t="s">
+      <c r="A183" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B183">
@@ -2800,7 +2962,7 @@
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="4" t="s">
+      <c r="A184" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B184">
@@ -2809,7 +2971,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="4" t="s">
+      <c r="A185" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B185">
@@ -2818,7 +2980,7 @@
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="4" t="s">
+      <c r="A186" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B186">
@@ -2827,7 +2989,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="4" t="s">
+      <c r="A187" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B187">
@@ -2836,7 +2998,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="4" t="s">
+      <c r="A188" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B188">
@@ -2845,7 +3007,7 @@
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="4" t="s">
+      <c r="A189" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B189">
@@ -2854,7 +3016,7 @@
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="4" t="s">
+      <c r="A190" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B190">
@@ -2863,7 +3025,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="4" t="s">
+      <c r="A191" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B191">
@@ -2872,7 +3034,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="4" t="s">
+      <c r="A192" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B192">
@@ -2881,7 +3043,7 @@
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="4" t="s">
+      <c r="A193" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B193">
@@ -2890,7 +3052,7 @@
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="4" t="s">
+      <c r="A194" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B194">
@@ -2899,7 +3061,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="4" t="s">
+      <c r="A195" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B195">
@@ -2908,7 +3070,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="4" t="s">
+      <c r="A196" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B196">
@@ -2917,7 +3079,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="4" t="s">
+      <c r="A197" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B197">
@@ -2926,7 +3088,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="4" t="s">
+      <c r="A198" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B198">
@@ -2935,7 +3097,7 @@
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="4" t="s">
+      <c r="A199" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B199">
@@ -2944,7 +3106,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="4" t="s">
+      <c r="A200" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B200">
@@ -2953,7 +3115,7 @@
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="4" t="s">
+      <c r="A201" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B201">
@@ -2962,7 +3124,7 @@
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="4" t="s">
+      <c r="A202" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B202">
@@ -2971,7 +3133,7 @@
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="4" t="s">
+      <c r="A203" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B203">
@@ -2980,7 +3142,7 @@
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="4" t="s">
+      <c r="A204" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B204">
@@ -2989,7 +3151,7 @@
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="4" t="s">
+      <c r="A205" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B205">
@@ -2998,7 +3160,7 @@
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="4" t="s">
+      <c r="A206" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B206">
@@ -3007,7 +3169,7 @@
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="4" t="s">
+      <c r="A207" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B207">
@@ -3016,7 +3178,7 @@
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="4" t="s">
+      <c r="A208" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B208">
@@ -3025,7 +3187,7 @@
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="4" t="s">
+      <c r="A209" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B209">
@@ -3034,7 +3196,7 @@
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="4" t="s">
+      <c r="A210" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B210">
@@ -3043,7 +3205,7 @@
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="4" t="s">
+      <c r="A211" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B211">
@@ -3052,7 +3214,7 @@
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="4" t="s">
+      <c r="A212" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B212">
@@ -3061,7 +3223,7 @@
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="4" t="s">
+      <c r="A213" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B213">
@@ -3070,7 +3232,7 @@
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="4" t="s">
+      <c r="A214" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B214">
@@ -3079,7 +3241,7 @@
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="4" t="s">
+      <c r="A215" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B215">
@@ -3088,7 +3250,7 @@
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="4" t="s">
+      <c r="A216" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B216">
@@ -3097,7 +3259,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="4" t="s">
+      <c r="A217" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B217">
@@ -3106,7 +3268,7 @@
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="4" t="s">
+      <c r="A218" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B218">
@@ -3115,7 +3277,7 @@
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="4" t="s">
+      <c r="A219" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B219">
@@ -3124,7 +3286,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="4" t="s">
+      <c r="A220" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B220">
@@ -3133,7 +3295,7 @@
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="4" t="s">
+      <c r="A221" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B221">
@@ -3142,7 +3304,7 @@
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="4" t="s">
+      <c r="A222" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B222">
@@ -3151,7 +3313,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="4" t="s">
+      <c r="A223" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B223">
@@ -3160,7 +3322,7 @@
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="4" t="s">
+      <c r="A224" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B224">
@@ -3169,7 +3331,7 @@
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="4" t="s">
+      <c r="A225" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B225">
@@ -3178,7 +3340,7 @@
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="4" t="s">
+      <c r="A226" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B226">
@@ -3187,7 +3349,7 @@
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="4" t="s">
+      <c r="A227" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B227">
@@ -3196,7 +3358,7 @@
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="4" t="s">
+      <c r="A228" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B228">
@@ -3205,7 +3367,7 @@
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="4" t="s">
+      <c r="A229" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B229">
@@ -3214,7 +3376,7 @@
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="4" t="s">
+      <c r="A230" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B230">
@@ -3223,7 +3385,7 @@
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="4" t="s">
+      <c r="A231" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B231">
@@ -3232,7 +3394,7 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="4" t="s">
+      <c r="A232" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B232">
@@ -3241,7 +3403,7 @@
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="5" t="s">
+      <c r="A233" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B233">
@@ -3250,7 +3412,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="5" t="s">
+      <c r="A234" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B234">
@@ -3259,7 +3421,7 @@
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="5" t="s">
+      <c r="A235" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B235">
@@ -3268,7 +3430,7 @@
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="5" t="s">
+      <c r="A236" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B236">
@@ -3277,7 +3439,7 @@
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="5" t="s">
+      <c r="A237" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B237">
@@ -3286,7 +3448,7 @@
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="5" t="s">
+      <c r="A238" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B238">
@@ -3295,7 +3457,7 @@
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="4" t="s">
+      <c r="A239" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B239">
@@ -3304,7 +3466,7 @@
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="4" t="s">
+      <c r="A240" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B240">
@@ -3313,7 +3475,7 @@
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="5" t="s">
+      <c r="A241" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B241">

</xml_diff>